<commit_message>
package assert response feature
</commit_message>
<xml_diff>
--- a/datas/platform.xlsx
+++ b/datas/platform.xlsx
@@ -67,7 +67,7 @@
     <t>{"username": "admin", "password": "123456"}</t>
   </si>
   <si>
-    <t>{"code": 0, "username": "admin"}</t>
+    <t>{"equal": {"code": 0, "username": "admin"}}</t>
   </si>
   <si>
     <t>except</t>
@@ -79,7 +79,7 @@
     <t>{"password": "123456"}</t>
   </si>
   <si>
-    <t>{"code": 1, "username": "该字段是必填项。"}</t>
+    <t>{"equal": {"code": 1}, "in": {"username": "该字段是必填项。"}}</t>
   </si>
   <si>
     <t>不传密码字段</t>
@@ -88,7 +88,7 @@
     <t>{"username": "admin"}</t>
   </si>
   <si>
-    <t>{"code": 1, "password": "该字段是必填项。"}</t>
+    <t>{"equal": {"code": 1}, "in": {"password": "该字段是必填项。"}}</t>
   </si>
   <si>
     <t>用户名为空</t>
@@ -97,7 +97,7 @@
     <t>{"username": "", "password": "123456"}</t>
   </si>
   <si>
-    <t>{"code": 1, "username": "该字段不能为空。"}</t>
+    <t>{"equal": {"code": 1}, "in": {"username": "该字段不能为空。"}}</t>
   </si>
   <si>
     <t>密码为空</t>
@@ -106,7 +106,7 @@
     <t>{"username": "admin", "password": ""}</t>
   </si>
   <si>
-    <t>{"code": 1, "password": "该字段不能为空。"}</t>
+    <t>{"equal": {"code": 1}, "in": {"password": "该字段不能为空。"}}</t>
   </si>
   <si>
     <t>用户名错误</t>
@@ -115,7 +115,7 @@
     <t>{"username": "ad123", "password": "123456"}</t>
   </si>
   <si>
-    <t>{"code": 1, "username": "账号错误。"}</t>
+    <t>{"equal": {"code": 1}, "in": {"username": "账号不存在！"}}</t>
   </si>
   <si>
     <t>密码错误</t>
@@ -124,7 +124,7 @@
     <t>{"username": "admin", "password": "666666"}</t>
   </si>
   <si>
-    <t>{"code": 1, "password": "密码错误。"}</t>
+    <t>{"equal": {"code": 1}, "in": {"password": "密码错误！"}}</t>
   </si>
 </sst>
 </file>
@@ -137,7 +137,7 @@
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,9 +161,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -175,27 +175,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -204,16 +189,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -242,6 +228,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -266,6 +260,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -276,22 +277,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -306,144 +299,180 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -451,42 +480,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -497,6 +490,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -580,15 +582,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -602,46 +595,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -650,109 +649,106 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1105,7 +1101,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7"/>
@@ -1115,7 +1111,7 @@
     <col min="5" max="5" width="14.625" customWidth="1"/>
     <col min="6" max="6" width="42.75" customWidth="1"/>
     <col min="9" max="9" width="44.375" customWidth="1"/>
-    <col min="10" max="10" width="46.25" customWidth="1"/>
+    <col min="10" max="10" width="80.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -1175,7 +1171,7 @@
       <c r="I2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="2" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
optimize case logic, and add detail run log
</commit_message>
<xml_diff>
--- a/datas/platform.xlsx
+++ b/datas/platform.xlsx
@@ -132,10 +132,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -154,30 +154,39 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -189,27 +198,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -254,7 +247,37 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -262,29 +285,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -299,187 +299,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -490,15 +490,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -513,6 +504,30 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -543,24 +558,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -582,11 +584,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -598,45 +598,48 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -646,97 +649,94 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>

</xml_diff>